<commit_message>
[Fix] Service.Catalog => Seed de catalogos (Falta etiquetas y modificar PK de EstudioParametro)
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/seed/04_CAT_INDICACIONES.xlsx
+++ b/Service.Catalog/wwwroot/seed/04_CAT_INDICACIONES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-71\source\repos\LaboratorioRamos\API\Service.Catalog\wwwroot\seed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB0EA7F-A132-4E20-984F-D52E9BAC2B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E9C3E5-6049-416F-93A9-3ADEF16B6FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INDICACIONES" sheetId="1" r:id="rId1"/>
@@ -759,7 +759,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -906,19 +906,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -987,7 +974,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1014,9 +1001,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1377,7 +1361,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,7 +1736,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>57</v>
@@ -1763,7 +1747,7 @@
     </row>
     <row r="35" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>59</v>
@@ -1774,7 +1758,7 @@
     </row>
     <row r="36" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>61</v>
@@ -1785,7 +1769,7 @@
     </row>
     <row r="37" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>63</v>
@@ -1796,7 +1780,7 @@
     </row>
     <row r="38" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>65</v>
@@ -1807,7 +1791,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>67</v>
@@ -1818,7 +1802,7 @@
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>68</v>
@@ -1829,7 +1813,7 @@
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>70</v>
@@ -1840,7 +1824,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>72</v>
@@ -1851,7 +1835,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>74</v>
@@ -1862,7 +1846,7 @@
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>76</v>
@@ -1873,7 +1857,7 @@
     </row>
     <row r="45" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>78</v>
@@ -1884,7 +1868,7 @@
     </row>
     <row r="46" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>80</v>
@@ -1895,7 +1879,7 @@
     </row>
     <row r="47" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>82</v>
@@ -1906,7 +1890,7 @@
     </row>
     <row r="48" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>84</v>
@@ -1917,7 +1901,7 @@
     </row>
     <row r="49" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>86</v>
@@ -1928,7 +1912,7 @@
     </row>
     <row r="50" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>88</v>
@@ -1939,7 +1923,7 @@
     </row>
     <row r="51" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>90</v>
@@ -1949,13 +1933,13 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="390" x14ac:dyDescent="0.25">
-      <c r="A52" s="8">
-        <v>47</v>
-      </c>
-      <c r="B52" s="9" t="s">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>